<commit_message>
add anonymous company name
</commit_message>
<xml_diff>
--- a/Data/Data Sander.xlsx
+++ b/Data/Data Sander.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isamu\Desktop\HvA Werk\Sander Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\GitHub\dashboard-zec\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57095C19-9191-408A-8F43-FA6E8D04940A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA9EBE1-9F60-4CBA-9ADD-22918FE3F8B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="170">
   <si>
     <t>Bedrijf</t>
   </si>
@@ -439,6 +439,99 @@
   </si>
   <si>
     <t>Goud</t>
+  </si>
+  <si>
+    <t>Bedrijf2</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>AD</t>
   </si>
 </sst>
 </file>
@@ -950,24 +1043,24 @@
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Berekening" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Controlecel" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Gekoppelde cel" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Goed" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Invoer" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Kop 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Kop 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Kop 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Kop 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Neutraal" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notitie" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Ongeldig" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
-    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Totaal" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Uitvoer" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Verklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Waarschuwingstekst" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -983,7 +1076,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1279,1382 +1372,1475 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV31"/>
+  <dimension ref="A1:AW31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="2" max="2" width="35.77734375" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
-    <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="27" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.5546875" customWidth="1"/>
+    <col min="3" max="3" width="35.77734375" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="27" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>135</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>108</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>109</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>110</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>111</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>27</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>31</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>32</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>33</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>34</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>35</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>36</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>37</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>38</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>39</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>40</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>43</v>
       </c>
       <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>46</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>136</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>48</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>49</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0</v>
-      </c>
-      <c r="L2">
-        <v>3</v>
       </c>
       <c r="M2">
         <v>3</v>
       </c>
-      <c r="O2">
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="P2">
         <v>90</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>30</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>75</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>50</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>12</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>3</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>16</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>11040</v>
       </c>
-      <c r="AH2">
+      <c r="AI2">
         <v>5500</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <v>37000</v>
       </c>
-      <c r="AJ2">
+      <c r="AK2">
         <v>216690</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>112</v>
       </c>
       <c r="B3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>51</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>52</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>136</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
       </c>
       <c r="H3" t="s">
         <v>48</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3">
         <v>40</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>70</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>90</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>2</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>3</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>16</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>11040</v>
       </c>
-      <c r="AB3">
+      <c r="AC3">
         <v>250</v>
       </c>
-      <c r="AE3">
+      <c r="AF3">
         <v>300</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>3380</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>12250</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <v>548524</v>
       </c>
-      <c r="AP3">
+      <c r="AQ3">
         <v>5</v>
       </c>
-      <c r="AS3">
+      <c r="AT3">
         <v>10</v>
       </c>
-      <c r="AV3">
+      <c r="AW3">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>53</v>
       </c>
       <c r="B4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" t="s">
         <v>54</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>52</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>137</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>49</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>48</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>16</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>5</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>600</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>600</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>55</v>
       </c>
       <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" t="s">
         <v>56</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>52</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>137</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>48</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>20</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>1</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
       <c r="B6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" t="s">
         <v>58</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>52</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>137</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>49</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>48</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>1</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>3</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>59</v>
       </c>
       <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" t="s">
         <v>127</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>61</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>47</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>136</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>48</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>49</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>100</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>3</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>45</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>5</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>40</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>140</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>105</v>
       </c>
-      <c r="AH7">
+      <c r="AI7">
         <v>48000</v>
       </c>
-      <c r="AL7">
+      <c r="AM7">
         <v>3</v>
       </c>
-      <c r="AO7">
+      <c r="AP7">
         <v>5</v>
       </c>
-      <c r="AR7">
+      <c r="AS7">
         <v>10</v>
       </c>
-      <c r="AU7">
+      <c r="AV7">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>62</v>
       </c>
       <c r="B8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" t="s">
         <v>113</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>63</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>64</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>47</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>136</v>
-      </c>
-      <c r="G8" t="s">
-        <v>48</v>
       </c>
       <c r="H8" t="s">
         <v>48</v>
       </c>
-      <c r="K8">
+      <c r="I8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8">
         <v>1</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>0.25</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>14</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>80</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>16</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>2</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>128</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>58880</v>
       </c>
-      <c r="AD8">
+      <c r="AE8">
         <v>75</v>
       </c>
-      <c r="AG8">
+      <c r="AH8">
         <v>400</v>
       </c>
-      <c r="AH8">
+      <c r="AI8">
         <v>10000</v>
       </c>
-      <c r="AI8">
+      <c r="AJ8">
         <v>12000</v>
       </c>
-      <c r="AJ8">
+      <c r="AK8">
         <v>200000</v>
       </c>
-      <c r="AQ8">
+      <c r="AR8">
         <v>1</v>
       </c>
-      <c r="AT8">
+      <c r="AU8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>65</v>
       </c>
       <c r="B9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" t="s">
         <v>66</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>47</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>137</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>49</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
       <c r="B10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" t="s">
         <v>68</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>45</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>69</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>47</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>136</v>
-      </c>
-      <c r="G10" t="s">
-        <v>48</v>
       </c>
       <c r="H10" t="s">
         <v>48</v>
       </c>
-      <c r="K10">
+      <c r="I10" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10">
         <v>1</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>20</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>5</v>
-      </c>
-      <c r="N10">
-        <v>30</v>
       </c>
       <c r="O10">
         <v>30</v>
       </c>
       <c r="P10">
+        <v>30</v>
+      </c>
+      <c r="Q10">
         <v>20</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>10</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>120</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>3</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>80</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>55200</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>12</v>
       </c>
-      <c r="AD10">
+      <c r="AE10">
         <v>10</v>
       </c>
-      <c r="AG10">
+      <c r="AH10">
         <v>150</v>
       </c>
-      <c r="AH10">
+      <c r="AI10">
         <v>30000</v>
       </c>
-      <c r="AI10">
+      <c r="AJ10">
         <v>60000</v>
       </c>
-      <c r="AJ10">
+      <c r="AK10">
         <v>134000</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>70</v>
       </c>
       <c r="B11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" t="s">
         <v>71</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>45</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>61</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>47</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>138</v>
-      </c>
-      <c r="G11" t="s">
-        <v>48</v>
       </c>
       <c r="H11" t="s">
         <v>48</v>
       </c>
-      <c r="I11">
+      <c r="I11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11">
         <v>8</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>2</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>6</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>40</v>
-      </c>
-      <c r="M11">
-        <v>10</v>
       </c>
       <c r="N11">
         <v>10</v>
       </c>
       <c r="O11">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="P11">
         <v>60</v>
       </c>
       <c r="Q11">
+        <v>60</v>
+      </c>
+      <c r="R11">
         <v>30</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>145</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>143</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>12</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>3</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <v>16</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <v>11040</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
         <v>350</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>200</v>
       </c>
-      <c r="AD11">
+      <c r="AE11">
         <v>150</v>
-      </c>
-      <c r="AE11">
-        <v>600</v>
       </c>
       <c r="AF11">
         <v>600</v>
       </c>
       <c r="AG11">
+        <v>600</v>
+      </c>
+      <c r="AH11">
         <v>450</v>
       </c>
-      <c r="AH11">
+      <c r="AI11">
         <v>10000</v>
       </c>
-      <c r="AI11">
+      <c r="AJ11">
         <v>18000</v>
       </c>
-      <c r="AJ11">
+      <c r="AK11">
         <v>2200000</v>
       </c>
-      <c r="AK11">
+      <c r="AL11">
         <v>2</v>
-      </c>
-      <c r="AL11">
-        <v>1</v>
       </c>
       <c r="AM11">
         <v>1</v>
       </c>
       <c r="AN11">
+        <v>1</v>
+      </c>
+      <c r="AO11">
         <v>6</v>
       </c>
-      <c r="AO11">
+      <c r="AP11">
         <v>2</v>
       </c>
-      <c r="AP11">
+      <c r="AQ11">
         <v>15</v>
       </c>
-      <c r="AQ11">
+      <c r="AR11">
         <v>6</v>
       </c>
-      <c r="AR11">
+      <c r="AS11">
         <v>2</v>
       </c>
-      <c r="AS11">
+      <c r="AT11">
         <v>20</v>
       </c>
-      <c r="AT11">
+      <c r="AU11">
         <v>6</v>
       </c>
-      <c r="AU11">
+      <c r="AV11">
         <v>2</v>
       </c>
-      <c r="AV11">
+      <c r="AW11">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>114</v>
       </c>
       <c r="B12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" t="s">
         <v>72</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>47</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>137</v>
-      </c>
-      <c r="G12" t="s">
-        <v>49</v>
       </c>
       <c r="H12" t="s">
         <v>49</v>
       </c>
-      <c r="L12">
+      <c r="I12" t="s">
+        <v>49</v>
+      </c>
+      <c r="M12">
         <v>40</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>73</v>
       </c>
       <c r="B13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" t="s">
         <v>74</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>63</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>64</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>52</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>136</v>
-      </c>
-      <c r="G13" t="s">
-        <v>48</v>
       </c>
       <c r="H13" t="s">
         <v>48</v>
       </c>
-      <c r="I13">
+      <c r="I13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13">
         <v>75</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>140</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>45</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>550</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>1090000</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <v>15</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>3</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>16</v>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <v>11040</v>
       </c>
-      <c r="AB13">
+      <c r="AC13">
         <v>400</v>
       </c>
-      <c r="AE13">
+      <c r="AF13">
         <v>500</v>
       </c>
-      <c r="AH13">
+      <c r="AI13">
         <v>100000</v>
       </c>
-      <c r="AI13">
+      <c r="AJ13">
         <v>170000</v>
       </c>
-      <c r="AJ13">
+      <c r="AK13">
         <v>5048348</v>
       </c>
-      <c r="AM13">
+      <c r="AN13">
         <v>7</v>
       </c>
-      <c r="AP13">
+      <c r="AQ13">
         <v>31</v>
       </c>
-      <c r="AS13">
+      <c r="AT13">
         <v>51</v>
       </c>
-      <c r="AV13">
+      <c r="AW13">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>75</v>
       </c>
       <c r="B14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14" t="s">
         <v>76</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>63</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>64</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>52</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>136</v>
-      </c>
-      <c r="G14" t="s">
-        <v>48</v>
       </c>
       <c r="H14" t="s">
         <v>48</v>
       </c>
-      <c r="I14">
+      <c r="I14" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14">
         <v>2</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>4</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>3</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>1</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>60</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>15</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>1700000</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <v>2</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <v>3</v>
       </c>
-      <c r="Z14">
+      <c r="AA14">
         <v>16</v>
       </c>
-      <c r="AA14">
+      <c r="AB14">
         <v>11040</v>
       </c>
-      <c r="AB14">
+      <c r="AC14">
         <v>111</v>
       </c>
-      <c r="AD14">
+      <c r="AE14">
         <v>67</v>
       </c>
-      <c r="AE14">
+      <c r="AF14">
         <v>250</v>
       </c>
-      <c r="AG14">
+      <c r="AH14">
         <v>500</v>
       </c>
-      <c r="AH14">
+      <c r="AI14">
         <v>6500</v>
       </c>
-      <c r="AI14">
+      <c r="AJ14">
         <v>12000</v>
       </c>
-      <c r="AJ14">
+      <c r="AK14">
         <v>2200000</v>
       </c>
-      <c r="AN14">
+      <c r="AO14">
         <v>2</v>
       </c>
-      <c r="AP14">
+      <c r="AQ14">
         <v>1</v>
       </c>
-      <c r="AQ14">
+      <c r="AR14">
         <v>3</v>
-      </c>
-      <c r="AR14">
-        <v>1</v>
       </c>
       <c r="AS14">
         <v>1</v>
       </c>
       <c r="AT14">
+        <v>1</v>
+      </c>
+      <c r="AU14">
         <v>3</v>
-      </c>
-      <c r="AU14">
-        <v>1</v>
       </c>
       <c r="AV14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AW14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>77</v>
       </c>
       <c r="B15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" t="s">
         <v>78</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>47</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>137</v>
-      </c>
-      <c r="G15" t="s">
-        <v>49</v>
       </c>
       <c r="H15" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>79</v>
       </c>
       <c r="B16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" t="s">
         <v>80</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>47</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>137</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>49</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>48</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>1</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>2</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>81</v>
       </c>
       <c r="B17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" t="s">
         <v>82</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>52</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>137</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>49</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>48</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>1</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>3</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>30</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>83</v>
       </c>
       <c r="B18" t="s">
+        <v>159</v>
+      </c>
+      <c r="C18" t="s">
         <v>84</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>52</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>137</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>49</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>48</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>15</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>25</v>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>85</v>
       </c>
       <c r="B19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C19" t="s">
         <v>86</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>52</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>137</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>49</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>48</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>12</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>87</v>
       </c>
       <c r="B20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" t="s">
         <v>88</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>52</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>137</v>
-      </c>
-      <c r="G20" t="s">
-        <v>49</v>
       </c>
       <c r="H20" t="s">
         <v>49</v>
       </c>
-      <c r="L20">
+      <c r="I20" t="s">
+        <v>49</v>
+      </c>
+      <c r="M20">
         <v>50</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>116</v>
       </c>
       <c r="B21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" t="s">
         <v>133</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>47</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>137</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>49</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>117</v>
       </c>
       <c r="B22" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" t="s">
         <v>134</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>47</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>137</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>49</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>118</v>
       </c>
       <c r="B23" t="s">
+        <v>152</v>
+      </c>
+      <c r="C23" t="s">
         <v>72</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>47</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>137</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>49</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>128</v>
       </c>
       <c r="B24" t="s">
+        <v>163</v>
+      </c>
+      <c r="C24" t="s">
         <v>129</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>47</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>137</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>49</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>119</v>
       </c>
       <c r="B25" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" t="s">
         <v>78</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>47</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>137</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>49</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>120</v>
       </c>
       <c r="B26" t="s">
+        <v>165</v>
+      </c>
+      <c r="C26" t="s">
         <v>60</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>47</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>137</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>49</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>121</v>
       </c>
       <c r="B27" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" t="s">
         <v>122</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>47</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>137</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>49</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>123</v>
       </c>
       <c r="B28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" t="s">
         <v>124</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>47</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>137</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>49</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>125</v>
       </c>
       <c r="B29" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" t="s">
         <v>126</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>47</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>137</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>49</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>130</v>
       </c>
       <c r="B30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" t="s">
         <v>66</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>47</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>137</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>49</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>131</v>
       </c>
       <c r="B31" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" t="s">
         <v>132</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>47</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>137</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>49</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>